<commit_message>
Added Tests for Text Screening and Custom Text Lists
</commit_message>
<xml_diff>
--- a/ContentModeratorSDK.Tests/data.xlsx
+++ b/ContentModeratorSDK.Tests/data.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bacon\OBO\WABASH\Src\ContentModeratorSdk\ContentModeratorSDK_V2\ContentModeratorSDK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\m2sdkv2\Microsoft.CognitiveServices.ContentModerator-Windows\ContentModeratorSDK.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="240"/>
   </bookViews>
   <sheets>
-    <sheet name="ScreenText" sheetId="9" r:id="rId1"/>
+    <sheet name="TermMatch" sheetId="9" r:id="rId1"/>
     <sheet name="IdentifyLanguage" sheetId="8" r:id="rId2"/>
     <sheet name="ImageMatch" sheetId="6" r:id="rId3"/>
     <sheet name="OCRImage" sheetId="4" r:id="rId4"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="145">
   <si>
     <t>DataType</t>
   </si>
@@ -238,18 +238,6 @@
     <t>Label</t>
   </si>
   <si>
-    <t>text/plain</t>
-  </si>
-  <si>
-    <t>text/html</t>
-  </si>
-  <si>
-    <t>text/markdown</t>
-  </si>
-  <si>
-    <t>text/xml</t>
-  </si>
-  <si>
     <t>AutoCorrect</t>
   </si>
   <si>
@@ -257,6 +245,228 @@
   </si>
   <si>
     <t>Pii</t>
+  </si>
+  <si>
+    <t>TermToAdd</t>
+  </si>
+  <si>
+    <t>TextToScreen</t>
+  </si>
+  <si>
+    <t>MatchTerm</t>
+  </si>
+  <si>
+    <t>UrlCount</t>
+  </si>
+  <si>
+    <t>awsed</t>
+  </si>
+  <si>
+    <t>I like to awsed</t>
+  </si>
+  <si>
+    <t>Plain</t>
+  </si>
+  <si>
+    <t>InputText</t>
+  </si>
+  <si>
+    <t>ExpectedLanguage</t>
+  </si>
+  <si>
+    <t>Hi this is how</t>
+  </si>
+  <si>
+    <t>你好你好吗</t>
+  </si>
+  <si>
+    <t>Chinese Simplified</t>
+  </si>
+  <si>
+    <t>你好你好嗎</t>
+  </si>
+  <si>
+    <t>Chinese Traditional</t>
+  </si>
+  <si>
+    <t>Ahoj jak se máš</t>
+  </si>
+  <si>
+    <t>Czech</t>
+  </si>
+  <si>
+    <t>Hallo hoe gaat het</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>Hei mitä kuuluu</t>
+  </si>
+  <si>
+    <t>Finnish</t>
+  </si>
+  <si>
+    <t>salut comment ca va</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Hallo, wie geht es dir</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>γεια πως εισαι</t>
+  </si>
+  <si>
+    <t>Szia hogy vagytok</t>
+  </si>
+  <si>
+    <t>Hungarian</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>Ciao, come stai</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>こんにちは、元気ですか</t>
+  </si>
+  <si>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>안녕 잘 지내</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Norwegian</t>
+  </si>
+  <si>
+    <t>cześć jak się masz</t>
+  </si>
+  <si>
+    <t>Polish</t>
+  </si>
+  <si>
+    <t>Oi como vai você</t>
+  </si>
+  <si>
+    <t>Portuguese</t>
+  </si>
+  <si>
+    <t>Привет, как дела</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>Hola! ¿Cómo estás</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Hej hur mår du</t>
+  </si>
+  <si>
+    <t>Swedish</t>
+  </si>
+  <si>
+    <t>Turkish</t>
+  </si>
+  <si>
+    <t>zho_chs</t>
+  </si>
+  <si>
+    <t>zho_cht</t>
+  </si>
+  <si>
+    <t>ces</t>
+  </si>
+  <si>
+    <t>swe</t>
+  </si>
+  <si>
+    <t>nld</t>
+  </si>
+  <si>
+    <t>fin</t>
+  </si>
+  <si>
+    <t>fra</t>
+  </si>
+  <si>
+    <t>deu</t>
+  </si>
+  <si>
+    <t>ell</t>
+  </si>
+  <si>
+    <t>hun</t>
+  </si>
+  <si>
+    <t>ita</t>
+  </si>
+  <si>
+    <t>por</t>
+  </si>
+  <si>
+    <t>rus</t>
+  </si>
+  <si>
+    <t>tur</t>
+  </si>
+  <si>
+    <t>jpn</t>
+  </si>
+  <si>
+    <t>kor</t>
+  </si>
+  <si>
+    <t>nor</t>
+  </si>
+  <si>
+    <t>pol</t>
+  </si>
+  <si>
+    <t>spa</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Merhaba nasılsın, bugün harika bir gün</t>
+  </si>
+  <si>
+    <t>Hei hvordan har du det, er det en flott dag i dag</t>
+  </si>
+  <si>
+    <t>awsed1</t>
+  </si>
+  <si>
+    <t>I like to awsed, 4256919508, me@123.com, http://microsoft.com</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address</t>
   </si>
 </sst>
 </file>
@@ -755,11 +965,14 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1116,149 +1329,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="12.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="69" style="3" customWidth="1"/>
-    <col min="4" max="8" width="16.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="3.85546875" style="2" customWidth="1"/>
-    <col min="10" max="11" width="19.28515625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="35.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="60" style="3" customWidth="1"/>
+    <col min="5" max="8" width="16.28515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10" style="3" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="M1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3">
-        <v>200</v>
-      </c>
-      <c r="K2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>139</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J3" s="3">
-        <v>200</v>
+        <v>140</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="K3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L3" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" s="3">
-        <v>200</v>
-      </c>
-      <c r="K4" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J5" s="3">
-        <v>200</v>
-      </c>
-      <c r="K5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3" t="b">
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1270,10 +1496,350 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="31" style="3" customWidth="1"/>
+    <col min="3" max="3" width="66.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,7 +1929,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
@@ -1392,7 +1958,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
@@ -1421,7 +1987,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
@@ -1450,7 +2016,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -1479,7 +2045,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
@@ -1508,7 +2074,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>13</v>
@@ -1537,7 +2103,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>13</v>
@@ -1566,7 +2132,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>13</v>
@@ -1595,7 +2161,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>13</v>
@@ -1624,7 +2190,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>14</v>
@@ -1653,7 +2219,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
@@ -1682,7 +2248,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
@@ -1711,7 +2277,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
@@ -1740,7 +2306,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>14</v>
@@ -1769,7 +2335,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
@@ -1798,7 +2364,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
@@ -1827,7 +2393,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
@@ -1856,7 +2422,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
@@ -1885,7 +2451,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
@@ -1914,7 +2480,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>22</v>
@@ -1946,7 +2512,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>22</v>
@@ -1978,7 +2544,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>22</v>
@@ -2010,7 +2576,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>22</v>
@@ -2042,7 +2608,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>22</v>
@@ -2074,7 +2640,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>22</v>
@@ -2106,7 +2672,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>22</v>
@@ -2138,7 +2704,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>22</v>
@@ -2170,7 +2736,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>22</v>
@@ -2202,7 +2768,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>22</v>
@@ -2234,7 +2800,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>33</v>
@@ -2266,7 +2832,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>33</v>
@@ -2298,7 +2864,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>33</v>
@@ -2330,7 +2896,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>33</v>
@@ -2362,7 +2928,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>33</v>
@@ -2394,7 +2960,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>33</v>
@@ -2426,7 +2992,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>33</v>
@@ -2458,7 +3024,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>33</v>
@@ -2490,7 +3056,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>33</v>
@@ -2522,1297 +3088,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I41" s="3">
-        <v>400</v>
-      </c>
-      <c r="J41" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K41" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L41" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L41"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="31.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="81" style="3" customWidth="1"/>
-    <col min="5" max="6" width="16.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="3.85546875" style="2" customWidth="1"/>
-    <col min="9" max="10" width="19.28515625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="35.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="25.5703125" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3">
-        <v>401</v>
-      </c>
-      <c r="G2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3">
-        <v>200</v>
-      </c>
-      <c r="J2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>200</v>
-      </c>
-      <c r="J3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3">
-        <v>200</v>
-      </c>
-      <c r="J4" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>200</v>
-      </c>
-      <c r="J5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3">
-        <v>200</v>
-      </c>
-      <c r="J6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>200</v>
-      </c>
-      <c r="J7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3">
-        <v>200</v>
-      </c>
-      <c r="J8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>200</v>
-      </c>
-      <c r="J9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="3">
-        <v>200</v>
-      </c>
-      <c r="J10" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="3">
-        <v>200</v>
-      </c>
-      <c r="J11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="3">
-        <v>200</v>
-      </c>
-      <c r="J12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="3">
-        <v>200</v>
-      </c>
-      <c r="J13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="3">
-        <v>200</v>
-      </c>
-      <c r="J14" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3">
-        <v>200</v>
-      </c>
-      <c r="J15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="3">
-        <v>200</v>
-      </c>
-      <c r="J16" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="3">
-        <v>200</v>
-      </c>
-      <c r="J17" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K17" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="3">
-        <v>200</v>
-      </c>
-      <c r="J18" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
-        <v>200</v>
-      </c>
-      <c r="J19" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L19" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <v>200</v>
-      </c>
-      <c r="J20" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L20" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="3">
-        <v>200</v>
-      </c>
-      <c r="J21" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L21" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="3">
-        <v>400</v>
-      </c>
-      <c r="J22" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L22" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="3">
-        <v>400</v>
-      </c>
-      <c r="J23" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K23" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L23" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" s="3">
-        <v>400</v>
-      </c>
-      <c r="J24" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K24" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L24" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G25" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3">
-        <v>400</v>
-      </c>
-      <c r="J25" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K25" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L25" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" s="3">
-        <v>400</v>
-      </c>
-      <c r="J26" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K26" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L26" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" s="3">
-        <v>400</v>
-      </c>
-      <c r="J27" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K27" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L27" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" s="3">
-        <v>400</v>
-      </c>
-      <c r="J28" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K28" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L28" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3">
-        <v>400</v>
-      </c>
-      <c r="J29" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K29" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L29" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G30" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" s="3">
-        <v>400</v>
-      </c>
-      <c r="J30" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K30" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L30" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I31" s="3">
-        <v>400</v>
-      </c>
-      <c r="J31" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K31" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L31" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" s="3">
-        <v>400</v>
-      </c>
-      <c r="J32" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K32" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L32" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I33" s="3">
-        <v>400</v>
-      </c>
-      <c r="J33" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K33" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L33" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G34" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I34" s="3">
-        <v>400</v>
-      </c>
-      <c r="J34" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K34" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L34" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I35" s="3">
-        <v>400</v>
-      </c>
-      <c r="J35" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K35" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L35" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I36" s="3">
-        <v>400</v>
-      </c>
-      <c r="J36" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K36" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L36" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I37" s="3">
-        <v>400</v>
-      </c>
-      <c r="J37" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K37" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L37" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I38" s="3">
-        <v>400</v>
-      </c>
-      <c r="J38" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K38" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L38" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I39" s="3">
-        <v>400</v>
-      </c>
-      <c r="J39" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K39" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L39" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G40" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I40" s="3">
-        <v>400</v>
-      </c>
-      <c r="J40" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K40" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L40" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>33</v>
@@ -3853,7 +3129,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A41"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3959,7 +3235,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -4000,7 +3276,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -4041,7 +3317,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -4082,7 +3358,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>63</v>
@@ -4123,7 +3399,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -4164,7 +3440,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -4205,7 +3481,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -4246,7 +3522,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -4287,7 +3563,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" s="3">
         <v>10</v>
@@ -4328,7 +3604,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" s="3">
         <v>11</v>
@@ -4369,7 +3645,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" s="3">
         <v>12</v>
@@ -4410,7 +3686,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" s="3">
         <v>13</v>
@@ -4451,7 +3727,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" s="3">
         <v>14</v>
@@ -4492,7 +3768,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>64</v>
@@ -4533,7 +3809,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" s="3">
         <v>16</v>
@@ -4574,7 +3850,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" s="3">
         <v>17</v>
@@ -4615,7 +3891,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" s="3">
         <v>18</v>
@@ -4656,7 +3932,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>65</v>
@@ -4697,7 +3973,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" s="3">
         <v>20</v>
@@ -4738,7 +4014,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>41</v>
@@ -4779,7 +4055,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>42</v>
@@ -4820,7 +4096,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>43</v>
@@ -4861,7 +4137,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>44</v>
@@ -4902,7 +4178,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>45</v>
@@ -4943,7 +4219,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>46</v>
@@ -4984,7 +4260,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>47</v>
@@ -5025,7 +4301,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>48</v>
@@ -5066,7 +4342,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>49</v>
@@ -5107,7 +4383,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>50</v>
@@ -5148,7 +4424,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>51</v>
@@ -5189,7 +4465,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>52</v>
@@ -5230,7 +4506,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>53</v>
@@ -5271,7 +4547,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>54</v>
@@ -5312,7 +4588,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>55</v>
@@ -5353,7 +4629,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>56</v>
@@ -5394,7 +4670,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>57</v>
@@ -5435,7 +4711,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>58</v>
@@ -5476,7 +4752,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>59</v>
@@ -5517,7 +4793,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>60</v>
@@ -5570,8 +4846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:H41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5648,7 +4924,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
@@ -5674,7 +4950,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
@@ -5700,7 +4976,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
@@ -5726,7 +5002,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -5752,7 +5028,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
@@ -5778,7 +5054,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>13</v>
@@ -5804,7 +5080,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>13</v>
@@ -5830,7 +5106,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>13</v>
@@ -5856,7 +5132,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>13</v>
@@ -5882,7 +5158,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>14</v>
@@ -5908,7 +5184,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
@@ -5934,7 +5210,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
@@ -5960,7 +5236,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
@@ -5986,7 +5262,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>14</v>
@@ -6012,7 +5288,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
@@ -6038,7 +5314,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
@@ -6064,7 +5340,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
@@ -6090,7 +5366,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
@@ -6116,7 +5392,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
@@ -6142,7 +5418,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>22</v>
@@ -6171,7 +5447,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>22</v>
@@ -6200,7 +5476,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>22</v>
@@ -6229,7 +5505,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>22</v>
@@ -6258,7 +5534,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>22</v>
@@ -6287,7 +5563,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>22</v>
@@ -6316,7 +5592,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>22</v>
@@ -6345,7 +5621,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>22</v>
@@ -6374,7 +5650,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>22</v>
@@ -6403,7 +5679,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>22</v>
@@ -6432,7 +5708,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>33</v>
@@ -6461,7 +5737,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>33</v>
@@ -6490,7 +5766,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>33</v>
@@ -6519,7 +5795,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>33</v>
@@ -6548,7 +5824,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>33</v>
@@ -6577,7 +5853,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>33</v>
@@ -6606,7 +5882,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>33</v>
@@ -6635,7 +5911,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>33</v>
@@ -6664,7 +5940,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>33</v>
@@ -6693,7 +5969,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>33</v>
@@ -6734,7 +6010,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6818,7 +6094,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
@@ -6847,7 +6123,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
@@ -6876,7 +6152,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
@@ -6905,7 +6181,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -6934,7 +6210,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
@@ -6963,7 +6239,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>13</v>
@@ -6992,7 +6268,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>13</v>
@@ -7021,7 +6297,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>13</v>
@@ -7050,7 +6326,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>13</v>
@@ -7079,7 +6355,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -7108,7 +6384,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
@@ -7137,7 +6413,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
@@ -7166,7 +6442,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
@@ -7195,7 +6471,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>14</v>
@@ -7224,7 +6500,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
@@ -7253,7 +6529,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
@@ -7282,7 +6558,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
@@ -7311,7 +6587,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
@@ -7340,7 +6616,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
@@ -7369,7 +6645,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>22</v>
@@ -7401,7 +6677,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>22</v>
@@ -7433,7 +6709,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>22</v>
@@ -7465,7 +6741,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>22</v>
@@ -7497,7 +6773,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>22</v>
@@ -7529,7 +6805,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>22</v>
@@ -7561,7 +6837,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>22</v>
@@ -7593,7 +6869,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>22</v>
@@ -7625,7 +6901,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>22</v>
@@ -7657,7 +6933,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>22</v>
@@ -7689,7 +6965,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>33</v>
@@ -7721,7 +6997,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>33</v>
@@ -7753,7 +7029,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>33</v>
@@ -7785,7 +7061,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>33</v>
@@ -7817,7 +7093,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>33</v>
@@ -7849,7 +7125,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>33</v>
@@ -7881,7 +7157,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>33</v>
@@ -7913,7 +7189,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>33</v>
@@ -7945,7 +7221,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>33</v>
@@ -7977,7 +7253,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>33</v>

</xml_diff>